<commit_message>
DungTT submit: Docs release for phase 1 - Core MQTT Broker
</commit_message>
<xml_diff>
--- a/Docs/Referrences/Masterplan.xlsx
+++ b/Docs/Referrences/Masterplan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1.Study\1.VGU\4.Semester_4\Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1.Study\1.VGU\4.Semester_4\MQTT_Broker_AkkaModel\Docs\Referrences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B33E3E-308E-4B2B-B34F-60E5DC72367F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA00FBD-4339-4BB0-A1F3-8686C67F7128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master plan" sheetId="2" r:id="rId1"/>
@@ -609,8 +609,22 @@
     <t>- Get 'SendingPacket' == valid packet (outbound) -&gt; decode -&gt; push in TCP stream</t>
   </si>
   <si>
-    <t>- FMS
-- Actor Model</t>
+    <r>
+      <t xml:space="preserve">- FMS
+- Actor Model
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Delay 2 weeks</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1706,8 +1720,8 @@
   </sheetPr>
   <dimension ref="A2:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1842,8 +1856,8 @@
       <c r="D7" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="20" t="s">
-        <v>10</v>
+      <c r="E7" s="18" t="s">
+        <v>7</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>32</v>
@@ -2408,8 +2422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E961F48-90F9-493A-BB41-64EF4EAD1B60}">
   <dimension ref="A2:G31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update report for web
</commit_message>
<xml_diff>
--- a/Docs/Referrences/Masterplan.xlsx
+++ b/Docs/Referrences/Masterplan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1.Study\1.VGU\4.Semester_4\MQTT_Broker_AkkaModel\Docs\Referrences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA00FBD-4339-4BB0-A1F3-8686C67F7128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED98DC7-815B-43B3-B7EB-182659A78FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master plan" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="130">
   <si>
     <t>No.</t>
   </si>
@@ -141,12 +141,6 @@
     <t>- Make sure user functions work as requires
 - Done related part in thesis report
 - Give a presentation to Prof</t>
-  </si>
-  <si>
-    <t>- Implement user's functions: (can be edited)
-+ Register for new device
-+ Show/hide values, status
-+ Errors report</t>
   </si>
   <si>
     <t>Take an overview about the topic:
@@ -625,6 +619,17 @@
       </rPr>
       <t>- Delay 2 weeks</t>
     </r>
+  </si>
+  <si>
+    <t>- Use Play Framework
+- Use AdminLTE 3</t>
+  </si>
+  <si>
+    <t>- Implement user's functions: (can be edited)
++ HTTP-MQTT convert
++ Register for new device
++ Show/hide values, status
++ Errors report</t>
   </si>
 </sst>
 </file>
@@ -1720,8 +1725,8 @@
   </sheetPr>
   <dimension ref="A2:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1756,7 +1761,7 @@
         <v>4</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1770,14 +1775,14 @@
         <v>6</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="72" x14ac:dyDescent="0.3">
@@ -1785,7 +1790,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>8</v>
@@ -1797,7 +1802,7 @@
         <v>7</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G4" s="28"/>
     </row>
@@ -1831,16 +1836,16 @@
         <v>12</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>47</v>
+        <v>64</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>7</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>28</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1863,10 +1868,10 @@
         <v>32</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -1877,10 +1882,10 @@
         <v>16</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>10</v>
+        <v>129</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>46</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>27</v>
@@ -1908,7 +1913,7 @@
       </c>
       <c r="G9" s="13"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -1919,13 +1924,13 @@
         <v>20</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>10</v>
+        <v>35</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>46</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>27</v>
+        <v>128</v>
       </c>
       <c r="G10" s="13"/>
     </row>
@@ -1940,7 +1945,7 @@
         <v>22</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>10</v>
@@ -2059,19 +2064,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>3</v>
@@ -2085,17 +2090,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G3" s="25" t="s">
         <v>7</v>
@@ -2107,17 +2112,17 @@
         <v>2</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G4" s="26" t="s">
         <v>7</v>
@@ -2131,15 +2136,15 @@
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
       <c r="D5" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="37"/>
       <c r="G5" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -2149,7 +2154,7 @@
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
       <c r="D6" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="37"/>
@@ -2165,7 +2170,7 @@
       <c r="B7" s="35"/>
       <c r="C7" s="35"/>
       <c r="D7" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="38"/>
@@ -2179,20 +2184,20 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="15" t="s">
         <v>58</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>59</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H8" s="13"/>
     </row>
@@ -2201,17 +2206,17 @@
         <v>7</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G9" s="26" t="s">
         <v>7</v>
@@ -2225,7 +2230,7 @@
       <c r="B10" s="30"/>
       <c r="C10" s="30"/>
       <c r="D10" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="32"/>
@@ -2239,23 +2244,23 @@
         <v>9</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2265,15 +2270,15 @@
       <c r="B12" s="30"/>
       <c r="C12" s="30"/>
       <c r="D12" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="32"/>
       <c r="G12" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2281,21 +2286,21 @@
         <v>11</v>
       </c>
       <c r="B13" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="C13" s="22" t="s">
-        <v>88</v>
-      </c>
       <c r="D13" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
       <c r="G13" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -2303,13 +2308,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="D14" s="15" t="s">
         <v>99</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>100</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -2323,13 +2328,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="D15" s="13" t="s">
         <v>102</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>103</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
@@ -2422,7 +2427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E961F48-90F9-493A-BB41-64EF4EAD1B60}">
   <dimension ref="A2:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -2440,27 +2445,27 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C2" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>69</v>
-      </c>
       <c r="F4" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>4</v>
@@ -2468,22 +2473,22 @@
     </row>
     <row r="5" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="5">
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>73</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>74</v>
       </c>
       <c r="G5" s="7"/>
     </row>
@@ -2493,16 +2498,16 @@
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G6" s="13"/>
     </row>
@@ -2512,16 +2517,16 @@
         <v>3</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="21" t="s">
-        <v>80</v>
-      </c>
       <c r="F7" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G7" s="7"/>
     </row>
@@ -2531,16 +2536,16 @@
         <v>4</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="E8" s="21" t="s">
-        <v>82</v>
-      </c>
       <c r="F8" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G8" s="13"/>
     </row>
@@ -2550,16 +2555,16 @@
         <v>5</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>75</v>
-      </c>
       <c r="F9" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G9" s="13"/>
     </row>
@@ -2569,37 +2574,37 @@
         <v>6</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>75</v>
-      </c>
       <c r="F10" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G10" s="13"/>
     </row>
     <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="5">
         <v>1</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>105</v>
-      </c>
       <c r="F11" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G11" s="13"/>
     </row>
@@ -2609,16 +2614,16 @@
         <v>2</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E12" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="E12" s="21" t="s">
-        <v>107</v>
-      </c>
       <c r="F12" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G12" s="13"/>
     </row>
@@ -2628,13 +2633,13 @@
         <v>3</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="13"/>
@@ -2645,16 +2650,16 @@
         <v>4</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G14" s="13"/>
     </row>
@@ -2664,16 +2669,16 @@
         <v>5</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="E15" s="21" t="s">
-        <v>113</v>
-      </c>
       <c r="F15" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G15" s="13"/>
     </row>
@@ -2683,16 +2688,16 @@
         <v>6</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G16" s="7"/>
     </row>
@@ -2702,16 +2707,16 @@
         <v>7</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G17" s="7"/>
     </row>
@@ -2721,16 +2726,16 @@
         <v>8</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G18" s="7"/>
     </row>
@@ -2740,16 +2745,16 @@
         <v>9</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G19" s="7"/>
     </row>
@@ -2759,16 +2764,16 @@
         <v>10</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="E20" s="21" t="s">
-        <v>120</v>
-      </c>
       <c r="F20" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G20" s="7"/>
     </row>
@@ -2778,16 +2783,16 @@
         <v>11</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G21" s="7"/>
     </row>
@@ -2797,16 +2802,16 @@
         <v>12</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G22" s="7"/>
     </row>
@@ -2816,14 +2821,14 @@
         <v>13</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E23" s="21"/>
       <c r="F23" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G23" s="7"/>
     </row>
@@ -2929,7 +2934,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>25</v>
@@ -2946,13 +2951,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="16">
         <v>44686</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>7</v>
@@ -2964,7 +2969,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="15"/>
@@ -2976,7 +2981,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="15"/>

</xml_diff>